<commit_message>
Added ability to return list of human players
Noticed a glitch that system only accepts names < 12 chars
</commit_message>
<xml_diff>
--- a/JavaFun/FlowDocumentation/MessageLayout.xlsx
+++ b/JavaFun/FlowDocumentation/MessageLayout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>Disconnect Message</t>
   </si>
@@ -354,8 +354,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -377,9 +383,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -424,6 +427,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,586 +725,605 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="12" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="31.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="28.42578125" style="3" customWidth="1"/>
-    <col min="12" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="27.28515625" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="2" max="2" width="12" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="5" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="5"/>
+    <col min="8" max="8" width="31.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="5"/>
+    <col min="11" max="11" width="28.42578125" style="5" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="5"/>
+    <col min="15" max="15" width="27.28515625" style="5" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="G2" s="18" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="G2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="20"/>
+      <c r="J2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="M2" s="15" t="s">
+      <c r="K2" s="11"/>
+      <c r="M2" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="G3" s="20" t="s">
+      <c r="E3" s="4"/>
+      <c r="G3" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="16" t="s">
+      <c r="M3" s="16"/>
+      <c r="N3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16" t="s">
+      <c r="O3" s="17"/>
+      <c r="P3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="16"/>
+      <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="G4" s="22" t="s">
+      <c r="E4" s="4"/>
+      <c r="G4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="16">
         <v>0</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16" t="s">
+      <c r="O4" s="17"/>
+      <c r="P4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="G5" s="22" t="s">
+      <c r="E5" s="4"/>
+      <c r="G5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="16">
         <v>1</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="16">
         <v>1</v>
       </c>
-      <c r="O5" s="15">
+      <c r="O5" s="16">
         <v>2</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="P5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="17"/>
+      <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:17" ht="30.75" thickBot="1">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="G6" s="22" t="s">
+      <c r="E6" s="6"/>
+      <c r="G6" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="16">
         <v>2</v>
       </c>
-      <c r="N6" s="15" t="s">
+      <c r="N6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="16"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="16">
         <v>3</v>
       </c>
-      <c r="N7" s="16" t="s">
+      <c r="N7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" thickBot="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="22" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="G8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="16">
         <v>4</v>
       </c>
-      <c r="N8" s="16" t="s">
+      <c r="N8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16" t="s">
+      <c r="O8" s="17"/>
+      <c r="P8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="16"/>
+      <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="G9" s="22" t="s">
+      <c r="E9" s="4"/>
+      <c r="G9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:17" ht="30">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>3</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="3" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>3</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>0</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>1</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="8">
+      <c r="A30" s="2">
         <v>6</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>7</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="8" t="s">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2"/>
+      <c r="B34" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2">
         <v>0</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1">
-        <v>40944</v>
-      </c>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2">
         <v>6</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E38" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="61">
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="N7:Q7"/>
     <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N8:O8"/>
@@ -1315,25 +1340,25 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="C28:E28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B19:C19"/>

</xml_diff>